<commit_message>
add gitignore and agg tab
</commit_message>
<xml_diff>
--- a/general_table.xlsx
+++ b/general_table.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,10 +473,15 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Mae</t>
+          <t>Mae old от pc</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mae pc от old </t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Тип данных</t>
         </is>
@@ -509,7 +514,10 @@
       <c r="H2" t="n">
         <v>20.79095465393795</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" t="n">
+        <v>20.79095465393795</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -542,7 +550,10 @@
       <c r="H3" t="n">
         <v>30.73508353221957</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="n">
+        <v>30.73508353221957</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -575,7 +586,10 @@
       <c r="H4" t="n">
         <v>34.98718377088306</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>34.98718377088306</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -608,7 +622,10 @@
       <c r="H5" t="n">
         <v>719.1622911694511</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" t="n">
+        <v>719.1622911694511</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -641,7 +658,10 @@
       <c r="H6" t="n">
         <v>29.91861575178998</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" t="n">
+        <v>29.91861575178998</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -674,7 +694,10 @@
       <c r="H7" t="n">
         <v>35.3008353221957</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" t="n">
+        <v>35.3008353221957</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -707,7 +730,10 @@
       <c r="H8" t="n">
         <v>2443.46062052506</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" t="n">
+        <v>2443.46062052506</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -740,7 +766,10 @@
       <c r="H9" t="n">
         <v>279.7808353221957</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" t="n">
+        <v>279.7808353221957</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -773,7 +802,10 @@
       <c r="H10" t="n">
         <v>224.8878281622912</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" t="n">
+        <v>224.8878281622912</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -806,7 +838,10 @@
       <c r="H11" t="n">
         <v>546.8806682577566</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" t="n">
+        <v>546.8806682577566</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -839,7 +874,10 @@
       <c r="H12" t="n">
         <v>1024.933174224344</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" t="n">
+        <v>1024.933174224344</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -872,7 +910,10 @@
       <c r="H13" t="n">
         <v>712.7303102625299</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>712.7303102625299</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -905,7 +946,10 @@
       <c r="H14" t="n">
         <v>1708.035799522673</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" t="n">
+        <v>1708.035799522673</v>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -938,7 +982,10 @@
       <c r="H15" t="n">
         <v>1476.940334128878</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" t="n">
+        <v>1476.940334128878</v>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -971,7 +1018,10 @@
       <c r="H16" t="n">
         <v>396.1026252983294</v>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I16" t="n">
+        <v>396.1026252983294</v>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1004,7 +1054,10 @@
       <c r="H17" t="n">
         <v>2113.579952267303</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I17" t="n">
+        <v>2113.579952267303</v>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1037,7 +1090,10 @@
       <c r="H18" t="n">
         <v>33.20525059665871</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" t="n">
+        <v>33.20525059665871</v>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -1070,7 +1126,10 @@
       <c r="H19" t="n">
         <v>21.3863245823389</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="n">
+        <v>21.3863245823389</v>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1103,7 +1162,10 @@
       <c r="H20" t="n">
         <v>34.6035799522673</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" t="n">
+        <v>34.6035799522673</v>
+      </c>
+      <c r="J20" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1136,7 +1198,10 @@
       <c r="H21" t="n">
         <v>34.91773269689737</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="n">
+        <v>34.91773269689737</v>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1169,7 +1234,10 @@
       <c r="H22" t="n">
         <v>34.64384725536993</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" t="n">
+        <v>34.64384725536993</v>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1202,7 +1270,10 @@
       <c r="H23" t="n">
         <v>35.31264916467781</v>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="I23" t="n">
+        <v>35.31264916467781</v>
+      </c>
+      <c r="J23" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -1235,7 +1306,10 @@
       <c r="H24" t="n">
         <v>35.42243436754177</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>35.42243436754177</v>
+      </c>
+      <c r="J24" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -1252,7 +1326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1298,10 +1372,15 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Mae</t>
+          <t>Mae old от pc</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mae pc от old </t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Тип данных</t>
         </is>
@@ -1310,31 +1389,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LF_HF_avg</t>
+          <t>RR_dev</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.02579182310134394</v>
+        <v>-0.5464594307314953</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5985715160246952</v>
+        <v>5.410051843408759e-34</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.05180102457911961</v>
+        <v>-0.5822574277186257</v>
       </c>
       <c r="E2" t="n">
-        <v>0.290108679579156</v>
+        <v>2.15404411724047e-39</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.02662321898582553</v>
+        <v>-0.3993450143072196</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4242631995883241</v>
+        <v>1.48569320693229e-32</v>
       </c>
       <c r="H2" t="n">
-        <v>32.74957040572793</v>
-      </c>
-      <c r="I2" t="inlineStr">
+        <v>27.4653937947494</v>
+      </c>
+      <c r="I2" t="n">
+        <v>27.4653937947494</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1343,31 +1425,34 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>MxDMn</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.051049313375385</v>
+        <v>-0.5435620472857288</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2971745733954062</v>
+        <v>1.387690786623231e-33</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.04418949121179205</v>
+        <v>-0.5929515160152762</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3669108416971257</v>
+        <v>3.86505080148962e-41</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.03127348488858941</v>
+        <v>-0.4081572919783005</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3733442679280212</v>
+        <v>1.910311440711857e-33</v>
       </c>
       <c r="H3" t="n">
-        <v>38.0090692124105</v>
-      </c>
-      <c r="I3" t="inlineStr">
+        <v>35.55634844868735</v>
+      </c>
+      <c r="I3" t="n">
+        <v>35.55634844868735</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1376,64 +1461,70 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>true_text_err</t>
+          <t>SDNN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1342774577987468</v>
+        <v>-0.5277838021174009</v>
       </c>
       <c r="C4" t="n">
-        <v>0.005907768282262114</v>
+        <v>2.003508019677792e-31</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0933664201855518</v>
+        <v>-0.5737733881637356</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05618129351874571</v>
+        <v>4.712914719282663e-38</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.07058624225013924</v>
+        <v>-0.3882730350532214</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05592617937964767</v>
+        <v>1.929998275894989e-31</v>
       </c>
       <c r="H4" t="n">
-        <v>34.25775656324582</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>discret</t>
+        <v>29.24931026252983</v>
+      </c>
+      <c r="I4" t="n">
+        <v>29.24931026252983</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>continious</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HF_dev</t>
+          <t>TP_avg</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2092853167880052</v>
+        <v>-0.5041172512759505</v>
       </c>
       <c r="C5" t="n">
-        <v>1.566749946239511e-05</v>
+        <v>2.166923696797284e-28</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4297245930996526</v>
+        <v>-0.6365479943168998</v>
       </c>
       <c r="E5" t="n">
-        <v>2.935824283059913e-20</v>
+        <v>5.541529363386069e-49</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2924744898074889</v>
+        <v>-0.4342626119152677</v>
       </c>
       <c r="G5" t="n">
-        <v>1.541564728541991e-18</v>
+        <v>6.644315376952809e-39</v>
       </c>
       <c r="H5" t="n">
-        <v>77.15102625298329</v>
-      </c>
-      <c r="I5" t="inlineStr">
+        <v>1208.710978520286</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1208.710978520286</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1442,31 +1533,34 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>VLF_dev</t>
+          <t>LF_avg</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2610646393766889</v>
+        <v>-0.4876518821887803</v>
       </c>
       <c r="C6" t="n">
-        <v>5.88671598775069e-08</v>
+        <v>2.04690511455362e-26</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.3709973480463336</v>
+        <v>-0.6679258802284073</v>
       </c>
       <c r="E6" t="n">
-        <v>4.047135078317819e-15</v>
+        <v>1.849104762046448e-55</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.2425354174832911</v>
+        <v>-0.4622239706924217</v>
       </c>
       <c r="G6" t="n">
-        <v>3.181580421115459e-13</v>
+        <v>7.640472282647523e-44</v>
       </c>
       <c r="H6" t="n">
-        <v>157.6442720763723</v>
-      </c>
-      <c r="I6" t="inlineStr">
+        <v>527.3847016706444</v>
+      </c>
+      <c r="I6" t="n">
+        <v>527.3847016706444</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1475,31 +1569,34 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TP_dev</t>
+          <t>HF_avg</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.2688022513164444</v>
+        <v>-0.4571903082758427</v>
       </c>
       <c r="C7" t="n">
-        <v>2.283810331495673e-08</v>
+        <v>4.952712345186693e-23</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.4680819771355473</v>
+        <v>-0.5609155582348924</v>
       </c>
       <c r="E7" t="n">
-        <v>3.339879121397265e-24</v>
+        <v>4.279172619233435e-36</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.3087336666320621</v>
+        <v>-0.3847075253368758</v>
       </c>
       <c r="G7" t="n">
-        <v>1.770812907494075e-20</v>
+        <v>6.75045048999236e-31</v>
       </c>
       <c r="H7" t="n">
-        <v>343.1267064439141</v>
-      </c>
-      <c r="I7" t="inlineStr">
+        <v>297.9373031026253</v>
+      </c>
+      <c r="I7" t="n">
+        <v>297.9373031026253</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1508,31 +1605,34 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LF_dev</t>
+          <t>HR_avg</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.3147592593044569</v>
+        <v>-0.4117401960933865</v>
       </c>
       <c r="C8" t="n">
-        <v>4.339223529442694e-11</v>
+        <v>1.416104026495604e-18</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.547878721956496</v>
+        <v>-0.4273205874398063</v>
       </c>
       <c r="E8" t="n">
-        <v>3.398987429115969e-34</v>
+        <v>4.996165778833412e-20</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3710461178551752</v>
+        <v>-0.3047470957125134</v>
       </c>
       <c r="G8" t="n">
-        <v>7.379491630090771e-29</v>
+        <v>1.357906087408714e-19</v>
       </c>
       <c r="H8" t="n">
-        <v>191.7767064439141</v>
-      </c>
-      <c r="I8" t="inlineStr">
+        <v>46.79474940334129</v>
+      </c>
+      <c r="I8" t="n">
+        <v>46.79474940334129</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1541,31 +1641,34 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.321426237561185</v>
+        <v>-0.3790104333203396</v>
       </c>
       <c r="C9" t="n">
-        <v>1.589989408773048e-11</v>
+        <v>9.223549217763994e-16</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.4567602375303867</v>
+        <v>-0.3816115256188788</v>
       </c>
       <c r="E9" t="n">
-        <v>5.498310724829417e-23</v>
+        <v>5.656877770123653e-16</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2981897739148267</v>
+        <v>-0.2930214606410836</v>
       </c>
       <c r="G9" t="n">
-        <v>3.530212730829705e-19</v>
+        <v>6.00925496607882e-15</v>
       </c>
       <c r="H9" t="n">
-        <v>35.75885441527446</v>
-      </c>
-      <c r="I9" t="inlineStr">
+        <v>45.23770883054893</v>
+      </c>
+      <c r="I9" t="n">
+        <v>45.23770883054893</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1574,31 +1677,34 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>pNN50</t>
+          <t>VLF_avg</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.3494574149852422</v>
+        <v>-0.3741128360219381</v>
       </c>
       <c r="C10" t="n">
-        <v>1.767014496350099e-13</v>
+        <v>2.288505699531055e-15</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.4183726704680148</v>
+        <v>-0.5118457498556842</v>
       </c>
       <c r="E10" t="n">
-        <v>3.483562455938237e-19</v>
+        <v>2.349959612806334e-29</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.2897425099769127</v>
+        <v>-0.3394521599212176</v>
       </c>
       <c r="G10" t="n">
-        <v>7.786466899237262e-18</v>
+        <v>2.019754988230423e-24</v>
       </c>
       <c r="H10" t="n">
-        <v>31.1108353221957</v>
-      </c>
-      <c r="I10" t="inlineStr">
+        <v>337.708138424821</v>
+      </c>
+      <c r="I10" t="n">
+        <v>337.708138424821</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1607,31 +1713,34 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>VLF_avg</t>
+          <t>pNN50</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.3741128360219381</v>
+        <v>-0.3494574149852422</v>
       </c>
       <c r="C11" t="n">
-        <v>2.288505699531055e-15</v>
+        <v>1.767014496350099e-13</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.5118457498556842</v>
+        <v>-0.4183726704680148</v>
       </c>
       <c r="E11" t="n">
-        <v>2.349959612806334e-29</v>
+        <v>3.483562455938237e-19</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.3394521599212176</v>
+        <v>-0.2897425099769127</v>
       </c>
       <c r="G11" t="n">
-        <v>2.019754988230423e-24</v>
+        <v>7.786466899237262e-18</v>
       </c>
       <c r="H11" t="n">
-        <v>337.708138424821</v>
-      </c>
-      <c r="I11" t="inlineStr">
+        <v>31.1108353221957</v>
+      </c>
+      <c r="I11" t="n">
+        <v>31.1108353221957</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1640,31 +1749,34 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.3790104333203396</v>
+        <v>-0.321426237561185</v>
       </c>
       <c r="C12" t="n">
-        <v>9.223549217763994e-16</v>
+        <v>1.589989408773048e-11</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.3816115256188788</v>
+        <v>-0.4567602375303867</v>
       </c>
       <c r="E12" t="n">
-        <v>5.656877770123653e-16</v>
+        <v>5.498310724829417e-23</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.2930214606410836</v>
+        <v>-0.2981897739148267</v>
       </c>
       <c r="G12" t="n">
-        <v>6.00925496607882e-15</v>
+        <v>3.530212730829705e-19</v>
       </c>
       <c r="H12" t="n">
-        <v>45.23770883054893</v>
-      </c>
-      <c r="I12" t="inlineStr">
+        <v>35.75885441527446</v>
+      </c>
+      <c r="I12" t="n">
+        <v>35.75885441527446</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1673,31 +1785,34 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HR_avg</t>
+          <t>LF_dev</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.4117401960933865</v>
+        <v>-0.3147592593044569</v>
       </c>
       <c r="C13" t="n">
-        <v>1.416104026495604e-18</v>
+        <v>4.339223529442694e-11</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.4273205874398063</v>
+        <v>-0.547878721956496</v>
       </c>
       <c r="E13" t="n">
-        <v>4.996165778833412e-20</v>
+        <v>3.398987429115969e-34</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.3047470957125134</v>
+        <v>-0.3710461178551752</v>
       </c>
       <c r="G13" t="n">
-        <v>1.357906087408714e-19</v>
+        <v>7.379491630090771e-29</v>
       </c>
       <c r="H13" t="n">
-        <v>46.79474940334129</v>
-      </c>
-      <c r="I13" t="inlineStr">
+        <v>191.7767064439141</v>
+      </c>
+      <c r="I13" t="n">
+        <v>191.7767064439141</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1706,31 +1821,34 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HF_avg</t>
+          <t>TP_dev</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.4571903082758427</v>
+        <v>-0.2688022513164444</v>
       </c>
       <c r="C14" t="n">
-        <v>4.952712345186693e-23</v>
+        <v>2.283810331495673e-08</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.5609155582348924</v>
+        <v>-0.4680819771355473</v>
       </c>
       <c r="E14" t="n">
-        <v>4.279172619233435e-36</v>
+        <v>3.339879121397265e-24</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.3847075253368758</v>
+        <v>-0.3087336666320621</v>
       </c>
       <c r="G14" t="n">
-        <v>6.75045048999236e-31</v>
+        <v>1.770812907494075e-20</v>
       </c>
       <c r="H14" t="n">
-        <v>297.9373031026253</v>
-      </c>
-      <c r="I14" t="inlineStr">
+        <v>343.1267064439141</v>
+      </c>
+      <c r="I14" t="n">
+        <v>343.1267064439141</v>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1739,31 +1857,34 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LF_avg</t>
+          <t>VLF_dev</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.4876518821887803</v>
+        <v>-0.2610646393766889</v>
       </c>
       <c r="C15" t="n">
-        <v>2.04690511455362e-26</v>
+        <v>5.88671598775069e-08</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.6679258802284073</v>
+        <v>-0.3709973480463336</v>
       </c>
       <c r="E15" t="n">
-        <v>1.849104762046448e-55</v>
+        <v>4.047135078317819e-15</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.4622239706924217</v>
+        <v>-0.2425354174832911</v>
       </c>
       <c r="G15" t="n">
-        <v>7.640472282647523e-44</v>
+        <v>3.181580421115459e-13</v>
       </c>
       <c r="H15" t="n">
-        <v>527.3847016706444</v>
-      </c>
-      <c r="I15" t="inlineStr">
+        <v>157.6442720763723</v>
+      </c>
+      <c r="I15" t="n">
+        <v>157.6442720763723</v>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1772,31 +1893,34 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TP_avg</t>
+          <t>HF_dev</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.5041172512759505</v>
+        <v>-0.2092853167880052</v>
       </c>
       <c r="C16" t="n">
-        <v>2.166923696797284e-28</v>
+        <v>1.566749946239511e-05</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.6365479943168998</v>
+        <v>-0.4297245930996526</v>
       </c>
       <c r="E16" t="n">
-        <v>5.541529363386069e-49</v>
+        <v>2.935824283059913e-20</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.4342626119152677</v>
+        <v>-0.2924744898074889</v>
       </c>
       <c r="G16" t="n">
-        <v>6.644315376952809e-39</v>
+        <v>1.541564728541991e-18</v>
       </c>
       <c r="H16" t="n">
-        <v>1208.710978520286</v>
-      </c>
-      <c r="I16" t="inlineStr">
+        <v>77.15102625298329</v>
+      </c>
+      <c r="I16" t="n">
+        <v>77.15102625298329</v>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1805,64 +1929,70 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SDNN</t>
+          <t>true_text_err</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.5277838021174009</v>
+        <v>-0.1342774577987468</v>
       </c>
       <c r="C17" t="n">
-        <v>2.003508019677792e-31</v>
+        <v>0.005907768282262114</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.5737733881637356</v>
+        <v>-0.0933664201855518</v>
       </c>
       <c r="E17" t="n">
-        <v>4.712914719282663e-38</v>
+        <v>0.05618129351874571</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.3882730350532214</v>
+        <v>-0.07058624225013924</v>
       </c>
       <c r="G17" t="n">
-        <v>1.929998275894989e-31</v>
+        <v>0.05592617937964767</v>
       </c>
       <c r="H17" t="n">
-        <v>29.24931026252983</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>continious</t>
+        <v>34.25775656324582</v>
+      </c>
+      <c r="I17" t="n">
+        <v>34.25775656324582</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>discret</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MxDMn</t>
+          <t>Q2</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.5435620472857288</v>
+        <v>-0.051049313375385</v>
       </c>
       <c r="C18" t="n">
-        <v>1.387690786623231e-33</v>
+        <v>0.2971745733954062</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.5929515160152762</v>
+        <v>-0.04418949121179205</v>
       </c>
       <c r="E18" t="n">
-        <v>3.86505080148962e-41</v>
+        <v>0.3669108416971257</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.4081572919783005</v>
+        <v>-0.03127348488858941</v>
       </c>
       <c r="G18" t="n">
-        <v>1.910311440711857e-33</v>
+        <v>0.3733442679280212</v>
       </c>
       <c r="H18" t="n">
-        <v>35.55634844868735</v>
-      </c>
-      <c r="I18" t="inlineStr">
+        <v>38.0090692124105</v>
+      </c>
+      <c r="I18" t="n">
+        <v>38.0090692124105</v>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1871,31 +2001,34 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RR_dev</t>
+          <t>LF_HF_avg</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.5464594307314953</v>
+        <v>-0.02579182310134394</v>
       </c>
       <c r="C19" t="n">
-        <v>5.410051843408759e-34</v>
+        <v>0.5985715160246952</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.5822574277186257</v>
+        <v>-0.05180102457911961</v>
       </c>
       <c r="E19" t="n">
-        <v>2.15404411724047e-39</v>
+        <v>0.290108679579156</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.3993450143072196</v>
+        <v>-0.02662321898582553</v>
       </c>
       <c r="G19" t="n">
-        <v>1.48569320693229e-32</v>
+        <v>0.4242631995883241</v>
       </c>
       <c r="H19" t="n">
-        <v>27.4653937947494</v>
-      </c>
-      <c r="I19" t="inlineStr">
+        <v>32.74957040572793</v>
+      </c>
+      <c r="I19" t="n">
+        <v>32.74957040572793</v>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -1912,7 +2045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1958,10 +2091,15 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Mae</t>
+          <t>Mae old от pc</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mae pc от old </t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Тип данных</t>
         </is>
@@ -1994,7 +2132,10 @@
       <c r="H2" t="n">
         <v>20.79095465393795</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" t="n">
+        <v>20.79095465393795</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2027,7 +2168,10 @@
       <c r="H3" t="n">
         <v>30.73508353221957</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="n">
+        <v>30.73508353221957</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -2060,7 +2204,10 @@
       <c r="H4" t="n">
         <v>34.98718377088306</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>34.98718377088306</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2093,7 +2240,10 @@
       <c r="H5" t="n">
         <v>719.1622911694511</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" t="n">
+        <v>719.1622911694511</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2126,7 +2276,10 @@
       <c r="H6" t="n">
         <v>29.91861575178998</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" t="n">
+        <v>29.91861575178998</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2159,7 +2312,10 @@
       <c r="H7" t="n">
         <v>35.3008353221957</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" t="n">
+        <v>35.3008353221957</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2192,7 +2348,10 @@
       <c r="H8" t="n">
         <v>2443.46062052506</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" t="n">
+        <v>2443.46062052506</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2225,7 +2384,10 @@
       <c r="H9" t="n">
         <v>279.7808353221957</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" t="n">
+        <v>279.7808353221957</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2258,7 +2420,10 @@
       <c r="H10" t="n">
         <v>224.8878281622912</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" t="n">
+        <v>224.8878281622912</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2291,7 +2456,10 @@
       <c r="H11" t="n">
         <v>546.8806682577566</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" t="n">
+        <v>546.8806682577566</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2324,7 +2492,10 @@
       <c r="H12" t="n">
         <v>1024.933174224344</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" t="n">
+        <v>1024.933174224344</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2357,7 +2528,10 @@
       <c r="H13" t="n">
         <v>712.7303102625299</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>712.7303102625299</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2390,7 +2564,10 @@
       <c r="H14" t="n">
         <v>1708.035799522673</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" t="n">
+        <v>1708.035799522673</v>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2423,7 +2600,10 @@
       <c r="H15" t="n">
         <v>1476.940334128878</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" t="n">
+        <v>1476.940334128878</v>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2456,7 +2636,10 @@
       <c r="H16" t="n">
         <v>396.1026252983294</v>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I16" t="n">
+        <v>396.1026252983294</v>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2489,7 +2672,10 @@
       <c r="H17" t="n">
         <v>2113.579952267303</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I17" t="n">
+        <v>2113.579952267303</v>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2522,7 +2708,10 @@
       <c r="H18" t="n">
         <v>33.20525059665871</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" t="n">
+        <v>33.20525059665871</v>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -2555,7 +2744,10 @@
       <c r="H19" t="n">
         <v>21.3863245823389</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="n">
+        <v>21.3863245823389</v>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2588,7 +2780,10 @@
       <c r="H20" t="n">
         <v>34.6035799522673</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" t="n">
+        <v>34.6035799522673</v>
+      </c>
+      <c r="J20" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2621,7 +2816,10 @@
       <c r="H21" t="n">
         <v>34.91773269689737</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="n">
+        <v>34.91773269689737</v>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2654,7 +2852,10 @@
       <c r="H22" t="n">
         <v>34.64384725536993</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" t="n">
+        <v>34.64384725536993</v>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2687,7 +2888,10 @@
       <c r="H23" t="n">
         <v>35.31264916467781</v>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="I23" t="n">
+        <v>35.31264916467781</v>
+      </c>
+      <c r="J23" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -2720,7 +2924,10 @@
       <c r="H24" t="n">
         <v>35.42243436754177</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>35.42243436754177</v>
+      </c>
+      <c r="J24" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -2753,7 +2960,10 @@
       <c r="H25" t="n">
         <v>32.74957040572793</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>32.74957040572793</v>
+      </c>
+      <c r="J25" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2786,7 +2996,10 @@
       <c r="H26" t="n">
         <v>38.0090692124105</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="I26" t="n">
+        <v>38.0090692124105</v>
+      </c>
+      <c r="J26" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2819,7 +3032,10 @@
       <c r="H27" t="n">
         <v>34.25775656324582</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" t="n">
+        <v>34.25775656324582</v>
+      </c>
+      <c r="J27" t="inlineStr">
         <is>
           <t>discret</t>
         </is>
@@ -2852,7 +3068,10 @@
       <c r="H28" t="n">
         <v>77.15102625298329</v>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="I28" t="n">
+        <v>77.15102625298329</v>
+      </c>
+      <c r="J28" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2885,7 +3104,10 @@
       <c r="H29" t="n">
         <v>157.6442720763723</v>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="I29" t="n">
+        <v>157.6442720763723</v>
+      </c>
+      <c r="J29" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2918,7 +3140,10 @@
       <c r="H30" t="n">
         <v>343.1267064439141</v>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="I30" t="n">
+        <v>343.1267064439141</v>
+      </c>
+      <c r="J30" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2951,7 +3176,10 @@
       <c r="H31" t="n">
         <v>191.7767064439141</v>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="I31" t="n">
+        <v>191.7767064439141</v>
+      </c>
+      <c r="J31" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -2984,7 +3212,10 @@
       <c r="H32" t="n">
         <v>35.75885441527446</v>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="I32" t="n">
+        <v>35.75885441527446</v>
+      </c>
+      <c r="J32" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3017,7 +3248,10 @@
       <c r="H33" t="n">
         <v>31.1108353221957</v>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" t="n">
+        <v>31.1108353221957</v>
+      </c>
+      <c r="J33" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3050,7 +3284,10 @@
       <c r="H34" t="n">
         <v>337.708138424821</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>337.708138424821</v>
+      </c>
+      <c r="J34" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3083,7 +3320,10 @@
       <c r="H35" t="n">
         <v>45.23770883054893</v>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="I35" t="n">
+        <v>45.23770883054893</v>
+      </c>
+      <c r="J35" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3116,7 +3356,10 @@
       <c r="H36" t="n">
         <v>46.79474940334129</v>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="I36" t="n">
+        <v>46.79474940334129</v>
+      </c>
+      <c r="J36" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3149,7 +3392,10 @@
       <c r="H37" t="n">
         <v>297.9373031026253</v>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="I37" t="n">
+        <v>297.9373031026253</v>
+      </c>
+      <c r="J37" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3182,7 +3428,10 @@
       <c r="H38" t="n">
         <v>527.3847016706444</v>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="I38" t="n">
+        <v>527.3847016706444</v>
+      </c>
+      <c r="J38" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3215,7 +3464,10 @@
       <c r="H39" t="n">
         <v>1208.710978520286</v>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="I39" t="n">
+        <v>1208.710978520286</v>
+      </c>
+      <c r="J39" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3248,7 +3500,10 @@
       <c r="H40" t="n">
         <v>29.24931026252983</v>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="I40" t="n">
+        <v>29.24931026252983</v>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3281,7 +3536,10 @@
       <c r="H41" t="n">
         <v>35.55634844868735</v>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="I41" t="n">
+        <v>35.55634844868735</v>
+      </c>
+      <c r="J41" t="inlineStr">
         <is>
           <t>continious</t>
         </is>
@@ -3314,7 +3572,10 @@
       <c r="H42" t="n">
         <v>27.4653937947494</v>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="I42" t="n">
+        <v>27.4653937947494</v>
+      </c>
+      <c r="J42" t="inlineStr">
         <is>
           <t>continious</t>
         </is>

</xml_diff>